<commit_message>
Updates adding HDV data in for vehicle revenue share by recipient ISIC code
</commit_message>
<xml_diff>
--- a/InputData/trans/VRSbRIC/Veh Revenue Share by Recipient ISIC Code.xlsx
+++ b/InputData/trans/VRSbRIC/Veh Revenue Share by Recipient ISIC Code.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\VRSbRIC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\trans\VRSbRIC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EF3998B-32D1-4235-8630-D2ADC701C06E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFABE065-4FE4-4AA3-B341-5EF8B4091819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{98104574-AC6C-45D3-B7DA-9D389A9BFE72}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{98104574-AC6C-45D3-B7DA-9D389A9BFE72}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="Data" sheetId="4" r:id="rId2"/>
-    <sheet name="VRSbRIC" sheetId="3" r:id="rId3"/>
+    <sheet name="LDV Data" sheetId="4" r:id="rId2"/>
+    <sheet name="HDV Data" sheetId="5" r:id="rId3"/>
+    <sheet name="VRSbRIC" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="133">
   <si>
     <t>VRSbRIC Vehicle Revenue Share by Recipient ISIC Code</t>
   </si>
@@ -413,6 +414,27 @@
   </si>
   <si>
     <t>The RPEF file also controls whether or not these values are used</t>
+  </si>
+  <si>
+    <t>Passenger LDVs</t>
+  </si>
+  <si>
+    <t>Freight LDVs and HDVs and Passenger HDVs</t>
+  </si>
+  <si>
+    <t>Heavy Duty Truck Retail Price Equivalent and Indirect Cost Multipliers</t>
+  </si>
+  <si>
+    <t>Manufacturing Cost</t>
+  </si>
+  <si>
+    <t>Dealer new vehicle net income</t>
+  </si>
+  <si>
+    <t>Dealer new vehicle selling expense</t>
+  </si>
+  <si>
+    <t>Trauck Manufacturers Industry Average</t>
   </si>
 </sst>
 </file>
@@ -471,7 +493,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -479,6 +501,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -535,6 +558,55 @@
         <a:xfrm>
           <a:off x="10086975" y="0"/>
           <a:ext cx="7913434" cy="5548617"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>541808</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>179557</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8E3DADF-2E71-3D63-AAEB-E30A6A4301EE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10725150" y="76200"/>
+          <a:ext cx="8933333" cy="11342857"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -843,10 +915,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA6E6C8E-C26C-4C73-93CC-7550EEEA6E9A}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,46 +935,82 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="3">
         <v>2009</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="3">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B21" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>125</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" xr:uid="{E18AB7C8-B002-4830-9F8F-289DE6D1CAE5}"/>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{E18AB7C8-B002-4830-9F8F-289DE6D1CAE5}"/>
+    <hyperlink ref="B14" r:id="rId2" xr:uid="{16F9FBDF-945F-40A7-8782-6520C8200155}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1522,6 +1630,619 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{289C64CC-E62D-4411-9368-8E9242EA44DA}">
+  <dimension ref="A1:E66"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="28.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>0.04</v>
+      </c>
+      <c r="D3">
+        <f>C3/($C$16-$C$2)</f>
+        <v>0.11111111111111102</v>
+      </c>
+      <c r="E3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>0.05</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D14" si="0">C4/($C$16-$C$2)</f>
+        <v>0.13888888888888878</v>
+      </c>
+      <c r="E4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>0.04</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0.11111111111111102</v>
+      </c>
+      <c r="E5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <v>0.02</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>5.5555555555555511E-2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>0.19444444444444428</v>
+      </c>
+      <c r="E7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <v>0.01</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>2.7777777777777755E-2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9">
+        <v>0.01</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>2.7777777777777755E-2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11">
+        <v>0.01</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>2.7777777777777755E-2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>131</v>
+      </c>
+      <c r="C13">
+        <v>0.06</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666652</v>
+      </c>
+      <c r="E13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s">
+        <v>111</v>
+      </c>
+      <c r="C14">
+        <v>0.05</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>0.13888888888888878</v>
+      </c>
+      <c r="E14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16">
+        <f>SUM(C2:C14)</f>
+        <v>1.3600000000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>75</v>
+      </c>
+      <c r="B30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>78</v>
+      </c>
+      <c r="B33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>79</v>
+      </c>
+      <c r="B34" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>80</v>
+      </c>
+      <c r="B35" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>82</v>
+      </c>
+      <c r="B37" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>83</v>
+      </c>
+      <c r="B38" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>84</v>
+      </c>
+      <c r="B39" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>86</v>
+      </c>
+      <c r="B41" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>87</v>
+      </c>
+      <c r="B42" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>88</v>
+      </c>
+      <c r="B43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>89</v>
+      </c>
+      <c r="B44" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>90</v>
+      </c>
+      <c r="B45" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>91</v>
+      </c>
+      <c r="B46" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>92</v>
+      </c>
+      <c r="B47" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>93</v>
+      </c>
+      <c r="B48" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>94</v>
+      </c>
+      <c r="B49" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>95</v>
+      </c>
+      <c r="B50" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>96</v>
+      </c>
+      <c r="B51" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>97</v>
+      </c>
+      <c r="B52" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>98</v>
+      </c>
+      <c r="B53" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>99</v>
+      </c>
+      <c r="B54" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>100</v>
+      </c>
+      <c r="B55" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>101</v>
+      </c>
+      <c r="B56" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>102</v>
+      </c>
+      <c r="B57" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>103</v>
+      </c>
+      <c r="B58" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>104</v>
+      </c>
+      <c r="B59" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>105</v>
+      </c>
+      <c r="B60" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>106</v>
+      </c>
+      <c r="B61" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>107</v>
+      </c>
+      <c r="B62" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>108</v>
+      </c>
+      <c r="B63" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>109</v>
+      </c>
+      <c r="B64" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>110</v>
+      </c>
+      <c r="B65" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>68</v>
+      </c>
+      <c r="B66" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F95DC9F-CBCD-437C-971E-4F1A6C1AB54A}">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
@@ -1529,7 +2250,7 @@
   <dimension ref="A1:AQ7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="X7" sqref="X7"/>
+      <selection activeCell="W7" sqref="W7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1673,171 +2394,171 @@
         <v>113</v>
       </c>
       <c r="B2">
-        <f>SUMIFS(Data!$D$3:$D$14,Data!$E$3:$E$14,B1)</f>
+        <f>SUMIFS('LDV Data'!$D$3:$D$14,'LDV Data'!$E$3:$E$14,B1)</f>
         <v>0</v>
       </c>
       <c r="C2">
-        <f>SUMIFS(Data!$D$3:$D$14,Data!$E$3:$E$14,C1)</f>
+        <f>SUMIFS('LDV Data'!$D$3:$D$14,'LDV Data'!$E$3:$E$14,C1)</f>
         <v>0</v>
       </c>
       <c r="D2">
-        <f>SUMIFS(Data!$D$3:$D$14,Data!$E$3:$E$14,D1)</f>
+        <f>SUMIFS('LDV Data'!$D$3:$D$14,'LDV Data'!$E$3:$E$14,D1)</f>
         <v>0</v>
       </c>
       <c r="E2">
-        <f>SUMIFS(Data!$D$3:$D$14,Data!$E$3:$E$14,E1)</f>
+        <f>SUMIFS('LDV Data'!$D$3:$D$14,'LDV Data'!$E$3:$E$14,E1)</f>
         <v>0</v>
       </c>
       <c r="F2">
-        <f>SUMIFS(Data!$D$3:$D$14,Data!$E$3:$E$14,F1)</f>
+        <f>SUMIFS('LDV Data'!$D$3:$D$14,'LDV Data'!$E$3:$E$14,F1)</f>
         <v>0</v>
       </c>
       <c r="G2">
-        <f>SUMIFS(Data!$D$3:$D$14,Data!$E$3:$E$14,G1)</f>
+        <f>SUMIFS('LDV Data'!$D$3:$D$14,'LDV Data'!$E$3:$E$14,G1)</f>
         <v>0</v>
       </c>
       <c r="H2">
-        <f>SUMIFS(Data!$D$3:$D$14,Data!$E$3:$E$14,H1)</f>
+        <f>SUMIFS('LDV Data'!$D$3:$D$14,'LDV Data'!$E$3:$E$14,H1)</f>
         <v>0</v>
       </c>
       <c r="I2">
-        <f>SUMIFS(Data!$D$3:$D$14,Data!$E$3:$E$14,I1)</f>
+        <f>SUMIFS('LDV Data'!$D$3:$D$14,'LDV Data'!$E$3:$E$14,I1)</f>
         <v>0</v>
       </c>
       <c r="J2">
-        <f>SUMIFS(Data!$D$3:$D$14,Data!$E$3:$E$14,J1)</f>
+        <f>SUMIFS('LDV Data'!$D$3:$D$14,'LDV Data'!$E$3:$E$14,J1)</f>
         <v>0</v>
       </c>
       <c r="K2">
-        <f>SUMIFS(Data!$D$3:$D$14,Data!$E$3:$E$14,K1)</f>
+        <f>SUMIFS('LDV Data'!$D$3:$D$14,'LDV Data'!$E$3:$E$14,K1)</f>
         <v>0</v>
       </c>
       <c r="L2">
-        <f>SUMIFS(Data!$D$3:$D$14,Data!$E$3:$E$14,L1)</f>
+        <f>SUMIFS('LDV Data'!$D$3:$D$14,'LDV Data'!$E$3:$E$14,L1)</f>
         <v>0</v>
       </c>
       <c r="M2">
-        <f>SUMIFS(Data!$D$3:$D$14,Data!$E$3:$E$14,M1)</f>
+        <f>SUMIFS('LDV Data'!$D$3:$D$14,'LDV Data'!$E$3:$E$14,M1)</f>
         <v>0</v>
       </c>
       <c r="N2">
-        <f>SUMIFS(Data!$D$3:$D$14,Data!$E$3:$E$14,N1)</f>
+        <f>SUMIFS('LDV Data'!$D$3:$D$14,'LDV Data'!$E$3:$E$14,N1)</f>
         <v>0</v>
       </c>
       <c r="O2">
-        <f>SUMIFS(Data!$D$3:$D$14,Data!$E$3:$E$14,O1)</f>
+        <f>SUMIFS('LDV Data'!$D$3:$D$14,'LDV Data'!$E$3:$E$14,O1)</f>
         <v>0</v>
       </c>
       <c r="P2">
-        <f>SUMIFS(Data!$D$3:$D$14,Data!$E$3:$E$14,P1)</f>
+        <f>SUMIFS('LDV Data'!$D$3:$D$14,'LDV Data'!$E$3:$E$14,P1)</f>
         <v>0</v>
       </c>
       <c r="Q2">
-        <f>SUMIFS(Data!$D$3:$D$14,Data!$E$3:$E$14,Q1)</f>
+        <f>SUMIFS('LDV Data'!$D$3:$D$14,'LDV Data'!$E$3:$E$14,Q1)</f>
         <v>0</v>
       </c>
       <c r="R2">
-        <f>SUMIFS(Data!$D$3:$D$14,Data!$E$3:$E$14,R1)</f>
+        <f>SUMIFS('LDV Data'!$D$3:$D$14,'LDV Data'!$E$3:$E$14,R1)</f>
         <v>0</v>
       </c>
       <c r="S2">
-        <f>SUMIFS(Data!$D$3:$D$14,Data!$E$3:$E$14,S1)</f>
+        <f>SUMIFS('LDV Data'!$D$3:$D$14,'LDV Data'!$E$3:$E$14,S1)</f>
         <v>0</v>
       </c>
       <c r="T2">
-        <f>SUMIFS(Data!$D$3:$D$14,Data!$E$3:$E$14,T1)</f>
+        <f>SUMIFS('LDV Data'!$D$3:$D$14,'LDV Data'!$E$3:$E$14,T1)</f>
         <v>0</v>
       </c>
       <c r="U2">
-        <f>SUMIFS(Data!$D$3:$D$14,Data!$E$3:$E$14,U1)</f>
+        <f>SUMIFS('LDV Data'!$D$3:$D$14,'LDV Data'!$E$3:$E$14,U1)</f>
         <v>0</v>
       </c>
       <c r="V2">
-        <f>SUMIFS(Data!$D$3:$D$14,Data!$E$3:$E$14,V1)</f>
+        <f>SUMIFS('LDV Data'!$D$3:$D$14,'LDV Data'!$E$3:$E$14,V1)</f>
         <v>0</v>
       </c>
       <c r="W2">
-        <f>SUMIFS(Data!$D$3:$D$14,Data!$E$3:$E$14,W1)</f>
+        <f>SUMIFS('LDV Data'!$D$3:$D$14,'LDV Data'!$E$3:$E$14,W1)</f>
         <v>0.6956521739130429</v>
       </c>
       <c r="X2">
-        <f>SUMIFS(Data!$D$3:$D$14,Data!$E$3:$E$14,X1)</f>
+        <f>SUMIFS('LDV Data'!$D$3:$D$14,'LDV Data'!$E$3:$E$14,X1)</f>
         <v>0</v>
       </c>
       <c r="Y2">
-        <f>SUMIFS(Data!$D$3:$D$14,Data!$E$3:$E$14,Y1)</f>
+        <f>SUMIFS('LDV Data'!$D$3:$D$14,'LDV Data'!$E$3:$E$14,Y1)</f>
         <v>0</v>
       </c>
       <c r="Z2">
-        <f>SUMIFS(Data!$D$3:$D$14,Data!$E$3:$E$14,Z1)</f>
+        <f>SUMIFS('LDV Data'!$D$3:$D$14,'LDV Data'!$E$3:$E$14,Z1)</f>
         <v>0</v>
       </c>
       <c r="AA2">
-        <f>SUMIFS(Data!$D$3:$D$14,Data!$E$3:$E$14,AA1)</f>
+        <f>SUMIFS('LDV Data'!$D$3:$D$14,'LDV Data'!$E$3:$E$14,AA1)</f>
         <v>0</v>
       </c>
       <c r="AB2">
-        <f>SUMIFS(Data!$D$3:$D$14,Data!$E$3:$E$14,AB1)</f>
+        <f>SUMIFS('LDV Data'!$D$3:$D$14,'LDV Data'!$E$3:$E$14,AB1)</f>
         <v>0</v>
       </c>
       <c r="AC2">
-        <f>SUMIFS(Data!$D$3:$D$14,Data!$E$3:$E$14,AC1)</f>
+        <f>SUMIFS('LDV Data'!$D$3:$D$14,'LDV Data'!$E$3:$E$14,AC1)</f>
         <v>0</v>
       </c>
       <c r="AD2">
-        <f>SUMIFS(Data!$D$3:$D$14,Data!$E$3:$E$14,AD1)</f>
+        <f>SUMIFS('LDV Data'!$D$3:$D$14,'LDV Data'!$E$3:$E$14,AD1)</f>
         <v>0.30434782608695626</v>
       </c>
       <c r="AE2">
-        <f>SUMIFS(Data!$D$3:$D$14,Data!$E$3:$E$14,AE1)</f>
+        <f>SUMIFS('LDV Data'!$D$3:$D$14,'LDV Data'!$E$3:$E$14,AE1)</f>
         <v>0</v>
       </c>
       <c r="AF2">
-        <f>SUMIFS(Data!$D$3:$D$14,Data!$E$3:$E$14,AF1)</f>
+        <f>SUMIFS('LDV Data'!$D$3:$D$14,'LDV Data'!$E$3:$E$14,AF1)</f>
         <v>0</v>
       </c>
       <c r="AG2">
-        <f>SUMIFS(Data!$D$3:$D$14,Data!$E$3:$E$14,AG1)</f>
+        <f>SUMIFS('LDV Data'!$D$3:$D$14,'LDV Data'!$E$3:$E$14,AG1)</f>
         <v>0</v>
       </c>
       <c r="AH2">
-        <f>SUMIFS(Data!$D$3:$D$14,Data!$E$3:$E$14,AH1)</f>
+        <f>SUMIFS('LDV Data'!$D$3:$D$14,'LDV Data'!$E$3:$E$14,AH1)</f>
         <v>0</v>
       </c>
       <c r="AI2">
-        <f>SUMIFS(Data!$D$3:$D$14,Data!$E$3:$E$14,AI1)</f>
+        <f>SUMIFS('LDV Data'!$D$3:$D$14,'LDV Data'!$E$3:$E$14,AI1)</f>
         <v>0</v>
       </c>
       <c r="AJ2">
-        <f>SUMIFS(Data!$D$3:$D$14,Data!$E$3:$E$14,AJ1)</f>
+        <f>SUMIFS('LDV Data'!$D$3:$D$14,'LDV Data'!$E$3:$E$14,AJ1)</f>
         <v>0</v>
       </c>
       <c r="AK2">
-        <f>SUMIFS(Data!$D$3:$D$14,Data!$E$3:$E$14,AK1)</f>
+        <f>SUMIFS('LDV Data'!$D$3:$D$14,'LDV Data'!$E$3:$E$14,AK1)</f>
         <v>0</v>
       </c>
       <c r="AL2">
-        <f>SUMIFS(Data!$D$3:$D$14,Data!$E$3:$E$14,AL1)</f>
+        <f>SUMIFS('LDV Data'!$D$3:$D$14,'LDV Data'!$E$3:$E$14,AL1)</f>
         <v>0</v>
       </c>
       <c r="AM2">
-        <f>SUMIFS(Data!$D$3:$D$14,Data!$E$3:$E$14,AM1)</f>
+        <f>SUMIFS('LDV Data'!$D$3:$D$14,'LDV Data'!$E$3:$E$14,AM1)</f>
         <v>0</v>
       </c>
       <c r="AN2">
-        <f>SUMIFS(Data!$D$3:$D$14,Data!$E$3:$E$14,AN1)</f>
+        <f>SUMIFS('LDV Data'!$D$3:$D$14,'LDV Data'!$E$3:$E$14,AN1)</f>
         <v>0</v>
       </c>
       <c r="AO2">
-        <f>SUMIFS(Data!$D$3:$D$14,Data!$E$3:$E$14,AO1)</f>
+        <f>SUMIFS('LDV Data'!$D$3:$D$14,'LDV Data'!$E$3:$E$14,AO1)</f>
         <v>0</v>
       </c>
       <c r="AP2">
-        <f>SUMIFS(Data!$D$3:$D$14,Data!$E$3:$E$14,AP1)</f>
+        <f>SUMIFS('LDV Data'!$D$3:$D$14,'LDV Data'!$E$3:$E$14,AP1)</f>
         <v>0</v>
       </c>
       <c r="AQ2">
-        <f>SUMIFS(Data!$D$3:$D$14,Data!$E$3:$E$14,AQ1)</f>
+        <f>SUMIFS('LDV Data'!$D$3:$D$14,'LDV Data'!$E$3:$E$14,AQ1)</f>
         <v>0</v>
       </c>
     </row>
@@ -1846,171 +2567,171 @@
         <v>114</v>
       </c>
       <c r="B3">
-        <f>B2</f>
+        <f>SUMIFS('HDV Data'!$D$3:$D$14,'HDV Data'!$E$3:$E$14,B1)</f>
         <v>0</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:AQ7" si="0">C2</f>
+        <f>SUMIFS('HDV Data'!$D$3:$D$14,'HDV Data'!$E$3:$E$14,C1)</f>
         <v>0</v>
       </c>
       <c r="D3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('HDV Data'!$D$3:$D$14,'HDV Data'!$E$3:$E$14,D1)</f>
         <v>0</v>
       </c>
       <c r="E3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('HDV Data'!$D$3:$D$14,'HDV Data'!$E$3:$E$14,E1)</f>
         <v>0</v>
       </c>
       <c r="F3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('HDV Data'!$D$3:$D$14,'HDV Data'!$E$3:$E$14,F1)</f>
         <v>0</v>
       </c>
       <c r="G3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('HDV Data'!$D$3:$D$14,'HDV Data'!$E$3:$E$14,G1)</f>
         <v>0</v>
       </c>
       <c r="H3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('HDV Data'!$D$3:$D$14,'HDV Data'!$E$3:$E$14,H1)</f>
         <v>0</v>
       </c>
       <c r="I3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('HDV Data'!$D$3:$D$14,'HDV Data'!$E$3:$E$14,I1)</f>
         <v>0</v>
       </c>
       <c r="J3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('HDV Data'!$D$3:$D$14,'HDV Data'!$E$3:$E$14,J1)</f>
         <v>0</v>
       </c>
       <c r="K3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('HDV Data'!$D$3:$D$14,'HDV Data'!$E$3:$E$14,K1)</f>
         <v>0</v>
       </c>
       <c r="L3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('HDV Data'!$D$3:$D$14,'HDV Data'!$E$3:$E$14,L1)</f>
         <v>0</v>
       </c>
       <c r="M3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('HDV Data'!$D$3:$D$14,'HDV Data'!$E$3:$E$14,M1)</f>
         <v>0</v>
       </c>
       <c r="N3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('HDV Data'!$D$3:$D$14,'HDV Data'!$E$3:$E$14,N1)</f>
         <v>0</v>
       </c>
       <c r="O3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('HDV Data'!$D$3:$D$14,'HDV Data'!$E$3:$E$14,O1)</f>
         <v>0</v>
       </c>
       <c r="P3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('HDV Data'!$D$3:$D$14,'HDV Data'!$E$3:$E$14,P1)</f>
         <v>0</v>
       </c>
       <c r="Q3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('HDV Data'!$D$3:$D$14,'HDV Data'!$E$3:$E$14,Q1)</f>
         <v>0</v>
       </c>
       <c r="R3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('HDV Data'!$D$3:$D$14,'HDV Data'!$E$3:$E$14,R1)</f>
         <v>0</v>
       </c>
       <c r="S3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('HDV Data'!$D$3:$D$14,'HDV Data'!$E$3:$E$14,S1)</f>
         <v>0</v>
       </c>
       <c r="T3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('HDV Data'!$D$3:$D$14,'HDV Data'!$E$3:$E$14,T1)</f>
         <v>0</v>
       </c>
       <c r="U3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('HDV Data'!$D$3:$D$14,'HDV Data'!$E$3:$E$14,U1)</f>
         <v>0</v>
       </c>
       <c r="V3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('HDV Data'!$D$3:$D$14,'HDV Data'!$E$3:$E$14,V1)</f>
         <v>0</v>
       </c>
       <c r="W3">
-        <f t="shared" si="0"/>
-        <v>0.6956521739130429</v>
+        <f>SUMIFS('HDV Data'!$D$3:$D$14,'HDV Data'!$E$3:$E$14,W1)</f>
+        <v>0.80555555555555491</v>
       </c>
       <c r="X3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('HDV Data'!$D$3:$D$14,'HDV Data'!$E$3:$E$14,X1)</f>
         <v>0</v>
       </c>
       <c r="Y3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('HDV Data'!$D$3:$D$14,'HDV Data'!$E$3:$E$14,Y1)</f>
         <v>0</v>
       </c>
       <c r="Z3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('HDV Data'!$D$3:$D$14,'HDV Data'!$E$3:$E$14,Z1)</f>
         <v>0</v>
       </c>
       <c r="AA3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('HDV Data'!$D$3:$D$14,'HDV Data'!$E$3:$E$14,AA1)</f>
         <v>0</v>
       </c>
       <c r="AB3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('HDV Data'!$D$3:$D$14,'HDV Data'!$E$3:$E$14,AB1)</f>
         <v>0</v>
       </c>
       <c r="AC3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('HDV Data'!$D$3:$D$14,'HDV Data'!$E$3:$E$14,AC1)</f>
         <v>0</v>
       </c>
       <c r="AD3">
-        <f t="shared" si="0"/>
-        <v>0.30434782608695626</v>
+        <f>SUMIFS('HDV Data'!$D$3:$D$14,'HDV Data'!$E$3:$E$14,AD1)</f>
+        <v>0.19444444444444428</v>
       </c>
       <c r="AE3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('HDV Data'!$D$3:$D$14,'HDV Data'!$E$3:$E$14,AE1)</f>
         <v>0</v>
       </c>
       <c r="AF3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('HDV Data'!$D$3:$D$14,'HDV Data'!$E$3:$E$14,AF1)</f>
         <v>0</v>
       </c>
       <c r="AG3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('HDV Data'!$D$3:$D$14,'HDV Data'!$E$3:$E$14,AG1)</f>
         <v>0</v>
       </c>
       <c r="AH3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('HDV Data'!$D$3:$D$14,'HDV Data'!$E$3:$E$14,AH1)</f>
         <v>0</v>
       </c>
       <c r="AI3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('HDV Data'!$D$3:$D$14,'HDV Data'!$E$3:$E$14,AI1)</f>
         <v>0</v>
       </c>
       <c r="AJ3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('HDV Data'!$D$3:$D$14,'HDV Data'!$E$3:$E$14,AJ1)</f>
         <v>0</v>
       </c>
       <c r="AK3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('HDV Data'!$D$3:$D$14,'HDV Data'!$E$3:$E$14,AK1)</f>
         <v>0</v>
       </c>
       <c r="AL3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('HDV Data'!$D$3:$D$14,'HDV Data'!$E$3:$E$14,AL1)</f>
         <v>0</v>
       </c>
       <c r="AM3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('HDV Data'!$D$3:$D$14,'HDV Data'!$E$3:$E$14,AM1)</f>
         <v>0</v>
       </c>
       <c r="AN3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('HDV Data'!$D$3:$D$14,'HDV Data'!$E$3:$E$14,AN1)</f>
         <v>0</v>
       </c>
       <c r="AO3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('HDV Data'!$D$3:$D$14,'HDV Data'!$E$3:$E$14,AO1)</f>
         <v>0</v>
       </c>
       <c r="AP3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('HDV Data'!$D$3:$D$14,'HDV Data'!$E$3:$E$14,AP1)</f>
         <v>0</v>
       </c>
       <c r="AQ3">
-        <f t="shared" si="0"/>
+        <f>SUMIFS('HDV Data'!$D$3:$D$14,'HDV Data'!$E$3:$E$14,AQ1)</f>
         <v>0</v>
       </c>
     </row>
@@ -2019,170 +2740,170 @@
         <v>115</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B7" si="1">B3</f>
+        <f t="shared" ref="B4:B7" si="0">B3</f>
         <v>0</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C3:AQ7" si="1">C3</f>
         <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W4" s="4">
         <v>0</v>
       </c>
       <c r="X4">
-        <f>W2</f>
-        <v>0.6956521739130429</v>
+        <f>W3</f>
+        <v>0.80555555555555491</v>
       </c>
       <c r="Y4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Z4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AB4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AC4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AD4">
-        <f t="shared" si="0"/>
-        <v>0.30434782608695626</v>
+        <f t="shared" si="1"/>
+        <v>0.19444444444444428</v>
       </c>
       <c r="AE4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AF4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AG4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AH4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AI4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AJ4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AK4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AL4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AM4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AN4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AO4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AP4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AQ4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2191,170 +2912,170 @@
         <v>116</v>
       </c>
       <c r="B5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W5" s="4">
         <v>0</v>
       </c>
       <c r="X5">
-        <f t="shared" si="0"/>
-        <v>0.6956521739130429</v>
+        <f t="shared" si="1"/>
+        <v>0.80555555555555491</v>
       </c>
       <c r="Y5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Z5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AB5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AC5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AD5">
-        <f t="shared" si="0"/>
-        <v>0.30434782608695626</v>
+        <f t="shared" si="1"/>
+        <v>0.19444444444444428</v>
       </c>
       <c r="AE5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AF5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AG5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AH5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AI5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AJ5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AK5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AL5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AM5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AN5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AO5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AP5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AQ5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2363,170 +3084,170 @@
         <v>117</v>
       </c>
       <c r="B6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W6" s="4">
         <v>0</v>
       </c>
       <c r="X6">
-        <f t="shared" si="0"/>
-        <v>0.6956521739130429</v>
+        <f t="shared" si="1"/>
+        <v>0.80555555555555491</v>
       </c>
       <c r="Y6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Z6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AB6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AC6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AD6">
-        <f t="shared" si="0"/>
-        <v>0.30434782608695626</v>
+        <f t="shared" si="1"/>
+        <v>0.19444444444444428</v>
       </c>
       <c r="AE6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AF6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AG6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AH6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AI6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AJ6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AK6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AL6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AM6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AN6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AO6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AP6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AQ6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2535,87 +3256,87 @@
         <v>118</v>
       </c>
       <c r="B7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W7">
@@ -2626,79 +3347,79 @@
         <v>0</v>
       </c>
       <c r="Y7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Z7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AB7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AC7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AD7">
-        <f t="shared" si="0"/>
-        <v>0.30434782608695626</v>
+        <f t="shared" si="1"/>
+        <v>0.19444444444444428</v>
       </c>
       <c r="AE7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AF7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AG7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AH7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AI7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AJ7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AK7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AL7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AM7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AN7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AO7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AP7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AQ7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>